<commit_message>
Modificaciones pp0008 y 0009 + excel guia
</commit_message>
<xml_diff>
--- a/Transparencia datos a descargar.xlsx
+++ b/Transparencia datos a descargar.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gusti\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\InfoLobby\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6BF465D-BBFC-49BE-94E1-A3CC8293F54A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15FA1AA4-3EF9-4145-8BFF-5F3463B7FF5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F45F3B4D-B921-4DAC-BE84-BD0E17A45B98}"/>
   </bookViews>
@@ -1748,8 +1748,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E32D1C0-6381-49D7-AEDF-A84C3FED8387}">
   <dimension ref="A1:M54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O7" sqref="O7"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="D50" sqref="D50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2269,7 +2269,7 @@
         <v>50</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E31" s="10" t="s">
         <v>175</v>
@@ -2286,7 +2286,7 @@
         <v>50</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E32" s="10" t="s">
         <v>176</v>
@@ -2303,7 +2303,7 @@
         <v>50</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E33" s="10" t="s">
         <v>177</v>
@@ -2320,7 +2320,7 @@
         <v>50</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E34" s="10" t="s">
         <v>178</v>
@@ -2337,7 +2337,7 @@
         <v>50</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E35" s="10" t="s">
         <v>179</v>
@@ -2354,7 +2354,7 @@
         <v>50</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E36" s="10" t="s">
         <v>180</v>
@@ -2370,8 +2370,8 @@
       <c r="C37" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="D37" s="7" t="s">
-        <v>10</v>
+      <c r="D37" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="E37" s="10" t="s">
         <v>181</v>
@@ -2387,8 +2387,8 @@
       <c r="C38" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="D38" s="7" t="s">
-        <v>10</v>
+      <c r="D38" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="E38" s="10" t="s">
         <v>182</v>
@@ -2404,8 +2404,8 @@
       <c r="C39" s="30" t="s">
         <v>50</v>
       </c>
-      <c r="D39" s="30" t="s">
-        <v>10</v>
+      <c r="D39" s="26" t="s">
+        <v>15</v>
       </c>
       <c r="E39" s="27" t="s">
         <v>183</v>
@@ -2426,8 +2426,8 @@
       <c r="C40" s="30" t="s">
         <v>50</v>
       </c>
-      <c r="D40" s="30" t="s">
-        <v>10</v>
+      <c r="D40" s="26" t="s">
+        <v>15</v>
       </c>
       <c r="E40" s="27" t="s">
         <v>184</v>
@@ -2448,8 +2448,8 @@
       <c r="C41" s="30" t="s">
         <v>50</v>
       </c>
-      <c r="D41" s="30" t="s">
-        <v>20</v>
+      <c r="D41" s="26" t="s">
+        <v>15</v>
       </c>
       <c r="E41" s="27" t="s">
         <v>185</v>
@@ -2470,8 +2470,8 @@
       <c r="C42" s="30" t="s">
         <v>50</v>
       </c>
-      <c r="D42" s="30" t="s">
-        <v>10</v>
+      <c r="D42" s="26" t="s">
+        <v>15</v>
       </c>
       <c r="E42" s="27" t="s">
         <v>186</v>
@@ -2492,8 +2492,8 @@
       <c r="C43" s="30" t="s">
         <v>50</v>
       </c>
-      <c r="D43" s="30" t="s">
-        <v>10</v>
+      <c r="D43" s="26" t="s">
+        <v>15</v>
       </c>
       <c r="E43" s="27" t="s">
         <v>187</v>
@@ -2514,8 +2514,8 @@
       <c r="C44" s="30" t="s">
         <v>50</v>
       </c>
-      <c r="D44" s="30" t="s">
-        <v>20</v>
+      <c r="D44" s="26" t="s">
+        <v>15</v>
       </c>
       <c r="E44" s="27" t="s">
         <v>188</v>
@@ -2536,8 +2536,8 @@
       <c r="C45" s="30" t="s">
         <v>50</v>
       </c>
-      <c r="D45" s="30" t="s">
-        <v>20</v>
+      <c r="D45" s="26" t="s">
+        <v>15</v>
       </c>
       <c r="E45" s="27" t="s">
         <v>189</v>
@@ -2558,8 +2558,8 @@
       <c r="C46" s="30" t="s">
         <v>50</v>
       </c>
-      <c r="D46" s="30" t="s">
-        <v>20</v>
+      <c r="D46" s="26" t="s">
+        <v>15</v>
       </c>
       <c r="E46" s="27" t="s">
         <v>190</v>
@@ -2580,8 +2580,8 @@
       <c r="C47" s="30" t="s">
         <v>50</v>
       </c>
-      <c r="D47" s="30" t="s">
-        <v>20</v>
+      <c r="D47" s="26" t="s">
+        <v>15</v>
       </c>
       <c r="E47" s="27" t="s">
         <v>191</v>
@@ -2602,8 +2602,8 @@
       <c r="C48" s="30" t="s">
         <v>50</v>
       </c>
-      <c r="D48" s="30" t="s">
-        <v>20</v>
+      <c r="D48" s="26" t="s">
+        <v>15</v>
       </c>
       <c r="E48" s="27" t="s">
         <v>192</v>
@@ -2624,8 +2624,8 @@
       <c r="C49" s="30" t="s">
         <v>50</v>
       </c>
-      <c r="D49" s="30" t="s">
-        <v>20</v>
+      <c r="D49" s="26" t="s">
+        <v>15</v>
       </c>
       <c r="E49" s="27" t="s">
         <v>193</v>
@@ -2646,8 +2646,8 @@
       <c r="C50" s="30" t="s">
         <v>50</v>
       </c>
-      <c r="D50" s="30" t="s">
-        <v>10</v>
+      <c r="D50" s="26" t="s">
+        <v>15</v>
       </c>
       <c r="E50" s="27" t="s">
         <v>194</v>

</xml_diff>